<commit_message>
added the residual plots
</commit_message>
<xml_diff>
--- a/results/Dashboard.xlsx
+++ b/results/Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TfL-Dataset\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899CD2B9-24EB-4649-975C-4BEE5B9AD5BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB2A406-A724-4369-9E89-7D9421E271BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E497BC3E-CC42-4FF6-8B84-CE96713D8523}"/>
   </bookViews>
@@ -6822,7 +6822,7 @@
   <dimension ref="D6:J13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>